<commit_message>
added code for descriptive plots and ran code
</commit_message>
<xml_diff>
--- a/data/Grouping Hospitalizations.xlsx
+++ b/data/Grouping Hospitalizations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10609"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joshh\Box\Hammer Lab\Current\Manuscripts\Paper Prep\1A. Ciitizen Paper\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kiran/Documents/GitHub/Ciitizen-health-scn8a/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69DFA2BB-826E-425B-917F-C6696A1BFC5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF38D2E8-CB74-4F45-BEF1-C9708172D4AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4340" yWindow="760" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -177,9 +177,6 @@
     <t>Planned</t>
   </si>
   <si>
-    <t>Admisison Type</t>
-  </si>
-  <si>
     <t>Type</t>
   </si>
   <si>
@@ -193,6 +190,9 @@
   </si>
   <si>
     <t>Unplanned</t>
+  </si>
+  <si>
+    <t>Admission Type</t>
   </si>
 </sst>
 </file>
@@ -512,30 +512,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A46" sqref="A46"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" t="s">
         <v>50</v>
-      </c>
-      <c r="B1" t="s">
-        <v>51</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B2" t="s">
         <v>48</v>
@@ -544,9 +542,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B3" t="s">
         <v>48</v>
@@ -555,7 +553,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>49</v>
       </c>
@@ -566,20 +564,20 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B6" t="s">
         <v>25</v>
@@ -588,7 +586,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>49</v>
       </c>
@@ -596,7 +594,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>49</v>
       </c>
@@ -604,9 +602,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B9" t="s">
         <v>48</v>
@@ -615,9 +613,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B10" t="s">
         <v>25</v>
@@ -626,7 +624,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>49</v>
       </c>
@@ -634,9 +632,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B12" t="s">
         <v>25</v>
@@ -645,9 +643,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B13" t="s">
         <v>48</v>
@@ -656,20 +654,20 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C14" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B15" t="s">
         <v>48</v>
@@ -678,53 +676,53 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B16" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C16" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B17" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C17" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B18" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C18" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B19" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C19" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B20" t="s">
         <v>48</v>
@@ -733,18 +731,18 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B21" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C21" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>49</v>
       </c>
@@ -752,20 +750,20 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B23" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C23" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B24" t="s">
         <v>48</v>
@@ -774,7 +772,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>49</v>
       </c>
@@ -782,9 +780,9 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B26" t="s">
         <v>25</v>
@@ -793,31 +791,31 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B27" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C27" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B28" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C28" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B29" t="s">
         <v>25</v>
@@ -826,62 +824,62 @@
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B30" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C30" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B31" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C31" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B32" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C32" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B33" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C33" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B34" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C34" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>49</v>
       </c>
@@ -889,31 +887,31 @@
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B36" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C36" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B37" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C37" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B38" t="s">
         <v>48</v>
@@ -922,31 +920,31 @@
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B39" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C39" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B40" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C40" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B41" t="s">
         <v>48</v>
@@ -955,20 +953,20 @@
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B42" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C42" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B43" t="s">
         <v>48</v>
@@ -977,9 +975,9 @@
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B44" t="s">
         <v>48</v>
@@ -988,7 +986,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>49</v>
       </c>
@@ -996,34 +994,34 @@
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B46" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C46" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B47" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C47" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B48" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C48" t="s">
         <v>47</v>

</xml_diff>

<commit_message>
Updated classifier and reran code for descriptive figures
</commit_message>
<xml_diff>
--- a/data/Grouping Hospitalizations.xlsx
+++ b/data/Grouping Hospitalizations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kiran/Documents/GitHub/Ciitizen-health-scn8a/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0064371-7607-8B47-AFA7-04A091071880}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17C080A9-A3F6-B542-AC05-AECA683C212E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4340" yWindow="760" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4340" yWindow="760" windowWidth="30220" windowHeight="20240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -192,9 +192,6 @@
     <t>Event</t>
   </si>
   <si>
-    <t>Unplanned</t>
-  </si>
-  <si>
     <t>Seizure</t>
   </si>
   <si>
@@ -226,6 +223,9 @@
   </si>
   <si>
     <t>Pulmonary</t>
+  </si>
+  <si>
+    <t>Incidental</t>
   </si>
   <si>
     <t>Admission Type</t>
@@ -244,12 +244,36 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -264,8 +288,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -548,7 +576,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D48"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -569,7 +599,7 @@
         <v>0</v>
       </c>
       <c r="D1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -583,7 +613,7 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -594,10 +624,10 @@
         <v>48</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>42</v>
       </c>
       <c r="D3" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -611,7 +641,7 @@
         <v>23</v>
       </c>
       <c r="D4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -622,10 +652,10 @@
         <v>48</v>
       </c>
       <c r="C5" t="s">
-        <v>42</v>
+        <v>12</v>
       </c>
       <c r="D5" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -639,7 +669,7 @@
         <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -653,7 +683,7 @@
         <v>9</v>
       </c>
       <c r="D7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -667,7 +697,7 @@
         <v>11</v>
       </c>
       <c r="D8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -677,11 +707,11 @@
       <c r="B9" t="s">
         <v>53</v>
       </c>
-      <c r="C9" t="s">
-        <v>13</v>
+      <c r="C9" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="D9" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -692,10 +722,10 @@
         <v>53</v>
       </c>
       <c r="C10" t="s">
-        <v>17</v>
+        <v>36</v>
       </c>
       <c r="D10" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -703,13 +733,13 @@
         <v>52</v>
       </c>
       <c r="B11" t="s">
-        <v>53</v>
-      </c>
-      <c r="C11" t="s">
-        <v>18</v>
+        <v>51</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="D11" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -723,7 +753,7 @@
         <v>20</v>
       </c>
       <c r="D12" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -731,13 +761,13 @@
         <v>52</v>
       </c>
       <c r="B13" t="s">
-        <v>53</v>
-      </c>
-      <c r="C13" t="s">
-        <v>30</v>
+        <v>51</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="D13" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -745,13 +775,13 @@
         <v>52</v>
       </c>
       <c r="B14" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C14" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="D14" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -765,7 +795,7 @@
         <v>39</v>
       </c>
       <c r="D15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -779,7 +809,7 @@
         <v>41</v>
       </c>
       <c r="D16" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -793,7 +823,7 @@
         <v>45</v>
       </c>
       <c r="D17" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -804,10 +834,10 @@
         <v>51</v>
       </c>
       <c r="C18" t="s">
-        <v>4</v>
+        <v>26</v>
       </c>
       <c r="D18" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -818,7 +848,7 @@
         <v>51</v>
       </c>
       <c r="C19" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="D19" t="s">
         <v>51</v>
@@ -831,8 +861,8 @@
       <c r="B20" t="s">
         <v>51</v>
       </c>
-      <c r="C20" t="s">
-        <v>16</v>
+      <c r="C20" s="1" t="s">
+        <v>31</v>
       </c>
       <c r="D20" t="s">
         <v>51</v>
@@ -845,8 +875,8 @@
       <c r="B21" t="s">
         <v>51</v>
       </c>
-      <c r="C21" t="s">
-        <v>22</v>
+      <c r="C21" s="1" t="s">
+        <v>33</v>
       </c>
       <c r="D21" t="s">
         <v>51</v>
@@ -860,10 +890,10 @@
         <v>51</v>
       </c>
       <c r="C22" t="s">
-        <v>26</v>
+        <v>46</v>
       </c>
       <c r="D22" t="s">
-        <v>51</v>
+        <v>64</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
@@ -873,8 +903,8 @@
       <c r="B23" t="s">
         <v>51</v>
       </c>
-      <c r="C23" t="s">
-        <v>27</v>
+      <c r="C23" s="2" t="s">
+        <v>47</v>
       </c>
       <c r="D23" t="s">
         <v>51</v>
@@ -885,13 +915,13 @@
         <v>52</v>
       </c>
       <c r="B24" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C24" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="D24" t="s">
-        <v>51</v>
+        <v>64</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
@@ -899,13 +929,13 @@
         <v>52</v>
       </c>
       <c r="B25" t="s">
-        <v>51</v>
-      </c>
-      <c r="C25" t="s">
-        <v>32</v>
-      </c>
-      <c r="D25" t="s">
-        <v>65</v>
+        <v>53</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
@@ -913,13 +943,13 @@
         <v>52</v>
       </c>
       <c r="B26" t="s">
-        <v>51</v>
-      </c>
-      <c r="C26" t="s">
-        <v>33</v>
-      </c>
-      <c r="D26" t="s">
-        <v>51</v>
+        <v>53</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
@@ -929,11 +959,11 @@
       <c r="B27" t="s">
         <v>51</v>
       </c>
-      <c r="C27" t="s">
-        <v>46</v>
+      <c r="C27" s="4" t="s">
+        <v>4</v>
       </c>
       <c r="D27" t="s">
-        <v>51</v>
+        <v>64</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
@@ -943,11 +973,11 @@
       <c r="B28" t="s">
         <v>51</v>
       </c>
-      <c r="C28" t="s">
-        <v>47</v>
+      <c r="C28" s="4" t="s">
+        <v>32</v>
       </c>
       <c r="D28" t="s">
-        <v>51</v>
+        <v>64</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
@@ -1019,7 +1049,7 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="B37" t="s">
         <v>48</v>
@@ -1028,12 +1058,12 @@
         <v>2</v>
       </c>
       <c r="D37" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="B38" t="s">
         <v>48</v>
@@ -1042,12 +1072,12 @@
         <v>8</v>
       </c>
       <c r="D38" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="B39" t="s">
         <v>48</v>
@@ -1056,12 +1086,12 @@
         <v>14</v>
       </c>
       <c r="D39" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="B40" t="s">
         <v>48</v>
@@ -1070,12 +1100,12 @@
         <v>19</v>
       </c>
       <c r="D40" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="B41" t="s">
         <v>25</v>
@@ -1084,12 +1114,12 @@
         <v>25</v>
       </c>
       <c r="D41" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="B42" t="s">
         <v>25</v>
@@ -1098,12 +1128,12 @@
         <v>28</v>
       </c>
       <c r="D42" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="B43" t="s">
         <v>53</v>
@@ -1112,12 +1142,12 @@
         <v>29</v>
       </c>
       <c r="D43" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="B44" t="s">
         <v>53</v>
@@ -1126,12 +1156,12 @@
         <v>35</v>
       </c>
       <c r="D44" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="B45" t="s">
         <v>48</v>
@@ -1140,12 +1170,12 @@
         <v>37</v>
       </c>
       <c r="D45" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="B46" t="s">
         <v>53</v>
@@ -1154,12 +1184,12 @@
         <v>38</v>
       </c>
       <c r="D46" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="B47" t="s">
         <v>48</v>
@@ -1168,12 +1198,12 @@
         <v>40</v>
       </c>
       <c r="D47" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="B48" t="s">
         <v>48</v>
@@ -1182,13 +1212,13 @@
         <v>43</v>
       </c>
       <c r="D48" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:E48" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C48">
-      <sortCondition ref="A1:A48"/>
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:D37">
+      <sortCondition ref="D1:D48"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>